<commit_message>
Tài liệu 348: 7613- Thêm tính năng mời Hội chẩn
</commit_message>
<xml_diff>
--- a/HIS/Plugins/HIS.Desktop.Plugins.ApprovaleDebate/zzz/HIS.Desktop.Plugins.ApprovaleDebate/Resources/ModuleKeyLanguage.xlsx
+++ b/HIS/Plugins/HIS.Desktop.Plugins.ApprovaleDebate/zzz/HIS.Desktop.Plugins.ApprovaleDebate/Resources/ModuleKeyLanguage.xlsx
@@ -185,6 +185,534 @@
   </si>
   <si>
     <t>တိုင်ပင်ဆွေးနွေး၏ခွင့်ပြုချက်</t>
+  </si>
+  <si>
+    <t>UCTreeListService.isRation.Caption</t>
+  </si>
+  <si>
+    <t>ĐTTT</t>
+  </si>
+  <si>
+    <t>đttt</t>
+  </si>
+  <si>
+    <t>UCTreeListService.layoutControl1.Text</t>
+  </si>
+  <si>
+    <t>UCTreeListService.tc_Delete.Caption</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>UCTreeListService.tc_Edit.Caption</t>
+  </si>
+  <si>
+    <t>UCTreeListService.tc_MediUsed.Caption</t>
+  </si>
+  <si>
+    <t>UCTreeListService.tc_NoteAdo.Caption</t>
+  </si>
+  <si>
+    <t>Ghi chú</t>
+  </si>
+  <si>
+    <t>Note</t>
+  </si>
+  <si>
+    <t>မှတ်ချက်</t>
+  </si>
+  <si>
+    <t>UCTreeListService.tc_Number.Caption</t>
+  </si>
+  <si>
+    <t>Số lượng</t>
+  </si>
+  <si>
+    <t>Quantity</t>
+  </si>
+  <si>
+    <t>အရေအတွက်</t>
+  </si>
+  <si>
+    <t>UCTreeListService.tc_RequestDepartmentName.Caption</t>
+  </si>
+  <si>
+    <t>Khoa yêu cầu</t>
+  </si>
+  <si>
+    <t>Faculty requires</t>
+  </si>
+  <si>
+    <t>ဒြေလိုအပ်သည်</t>
+  </si>
+  <si>
+    <t>UCTreeListService.tc_SendTestServiceReq.Caption</t>
+  </si>
+  <si>
+    <t>UCTreeListService.tc_ServiceCode.Caption</t>
+  </si>
+  <si>
+    <t>Mã dịch vụ</t>
+  </si>
+  <si>
+    <t>Service code</t>
+  </si>
+  <si>
+    <t>ဝန်ဆောင်မှုကုဒ်</t>
+  </si>
+  <si>
+    <t>UCTreeListService.tc_ServiceName.Caption</t>
+  </si>
+  <si>
+    <t>Tên dịch vụ</t>
+  </si>
+  <si>
+    <t>Service name</t>
+  </si>
+  <si>
+    <t>ဝန်ဆောင်မှုအမည်</t>
+  </si>
+  <si>
+    <t>UCTreeListService.tc_TdlMedicineConcentra.Caption</t>
+  </si>
+  <si>
+    <t>Hàm lượng</t>
+  </si>
+  <si>
+    <t>Content</t>
+  </si>
+  <si>
+    <t>ကေြနပ်သော</t>
+  </si>
+  <si>
+    <t>UCTreeListService.treeListColumn1.Caption</t>
+  </si>
+  <si>
+    <t>UCTreeListService.treeListColumn2.Caption</t>
+  </si>
+  <si>
+    <t>UCTreeListService.treeSereServ.OptionsFind.FindNullPrompt</t>
+  </si>
+  <si>
+    <t>Nhập chuỗi tìm kiếm ...</t>
+  </si>
+  <si>
+    <t>Enter the search string...</t>
+  </si>
+  <si>
+    <t>ရှာဖွေရေး string ကိုရိုက်ထည့်ပါ။</t>
+  </si>
+  <si>
+    <t>UCTreeListTracking.CONTENT.Caption</t>
+  </si>
+  <si>
+    <t>Diễn biến</t>
+  </si>
+  <si>
+    <t>Evolution</t>
+  </si>
+  <si>
+    <t>အဆင့်ဆင့်ဖြစ်ပျက်ခြင်း</t>
+  </si>
+  <si>
+    <t>UCTreeListTracking.layoutControl1.Text</t>
+  </si>
+  <si>
+    <t>UCTreeListTracking.SERVICE.Caption</t>
+  </si>
+  <si>
+    <t>Y lệnh</t>
+  </si>
+  <si>
+    <t>Command</t>
+  </si>
+  <si>
+    <t>အမိန့်</t>
+  </si>
+  <si>
+    <t>UCTreeListTracking.TRACKING_TIME.Caption</t>
+  </si>
+  <si>
+    <t>Ngày giờ</t>
+  </si>
+  <si>
+    <t>Dates and time</t>
+  </si>
+  <si>
+    <t>ရက်စွဲများနှင့်အချိန်</t>
+  </si>
+  <si>
+    <t>UCTreeListTracking.treeSereServ.OptionsFind.FindNullPrompt</t>
+  </si>
+  <si>
+    <t>UCTreeListTracking.USER_NAME.Caption</t>
+  </si>
+  <si>
+    <t>Bác sĩ</t>
+  </si>
+  <si>
+    <t>Doctor</t>
+  </si>
+  <si>
+    <t>ဆရာဝန်မ</t>
+  </si>
+  <si>
+    <t>BenhNhanCapCuu</t>
+  </si>
+  <si>
+    <t>Bệnh nhân cấp cứu</t>
+  </si>
+  <si>
+    <t>Emergency patient</t>
+  </si>
+  <si>
+    <t>အရေးပေါ်လူနာ</t>
+  </si>
+  <si>
+    <t>BenhNhanDaDuDieuKienRaVien</t>
+  </si>
+  <si>
+    <t>Bệnh nhân đã duyệt đủ điều kiện ra viện.</t>
+  </si>
+  <si>
+    <t>The patient was approved to be discharged from the hospital.</t>
+  </si>
+  <si>
+    <t>လူနာအား ဆေးရုံမှ ဆင်းခွင့်ပြုခဲ့သည်။</t>
+  </si>
+  <si>
+    <t>BHYT</t>
+  </si>
+  <si>
+    <t>BHYT: {0}/ {1}</t>
+  </si>
+  <si>
+    <t>Health Insurance: {0}/ {1}</t>
+  </si>
+  <si>
+    <t>ကျန်းမာရေးအာမခံ: {0}/ {1}</t>
+  </si>
+  <si>
+    <t>BNChuaKeDonTrongKhoang</t>
+  </si>
+  <si>
+    <t>BN chưa kê đơn trong khoảng</t>
+  </si>
+  <si>
+    <t>The patient has not prescribed for approx</t>
+  </si>
+  <si>
+    <t>လူနာသည် ခန့်မှန်းချေကို မသတ်မှတ်ထားပေ။</t>
+  </si>
+  <si>
+    <t>BNDangOTrongBuong</t>
+  </si>
+  <si>
+    <t>BN đang ở trong buồng</t>
+  </si>
+  <si>
+    <t>Patient is in the room</t>
+  </si>
+  <si>
+    <t>လူနာက အခန်းထဲမှာ</t>
+  </si>
+  <si>
+    <t>BNVaoTrongKhoang</t>
+  </si>
+  <si>
+    <t>BN vào trong khoảng</t>
+  </si>
+  <si>
+    <t>Patient is within</t>
+  </si>
+  <si>
+    <t>လူနာက အထဲမှာရှိတယ်။</t>
+  </si>
+  <si>
+    <t>CoBenhNhanhBHYTTrongTongSoBenhNhan</t>
+  </si>
+  <si>
+    <t>Có {0} bệnh nhân BHYT trong tổng số {1} bệnh nhân</t>
+  </si>
+  <si>
+    <t>There are {0} insured patients out of {1} patients</t>
+  </si>
+  <si>
+    <t>လူနာ {1} ဦးအနက် အာမခံထားသူ {0} ဦး ရှိပါသည်။</t>
+  </si>
+  <si>
+    <t>DaKetThucDieuTri</t>
+  </si>
+  <si>
+    <t>Đã kết thúc điều trị</t>
+  </si>
+  <si>
+    <t>Finished treatment</t>
+  </si>
+  <si>
+    <t>ကုသမှုပြီးပါပြီ။</t>
+  </si>
+  <si>
+    <t>DangDieuTriNgoaiBuong</t>
+  </si>
+  <si>
+    <t>Đang điều trị ngoài buồng</t>
+  </si>
+  <si>
+    <t>Treating out of the room</t>
+  </si>
+  <si>
+    <t>အခန်းထဲက ကုသပေးနေတယ်။</t>
+  </si>
+  <si>
+    <t>DangDieuTriTrongBuong</t>
+  </si>
+  <si>
+    <t>Đang điều trị trong buồng</t>
+  </si>
+  <si>
+    <t>Treating in the room</t>
+  </si>
+  <si>
+    <t>အခန်းထဲမှာ ဆေးကုတယ်။</t>
+  </si>
+  <si>
+    <t>DieuTriKetHop</t>
+  </si>
+  <si>
+    <t>Điều trị kết hợp</t>
+  </si>
+  <si>
+    <t>Combination treatment</t>
+  </si>
+  <si>
+    <t>ပေါင်းစပ်ကုသမှု</t>
+  </si>
+  <si>
+    <t>DieuTriThuong</t>
+  </si>
+  <si>
+    <t>Điều trị thường</t>
+  </si>
+  <si>
+    <t>Normal treatment</t>
+  </si>
+  <si>
+    <t>ပုံမှန်ကုသမှု</t>
+  </si>
+  <si>
+    <t>DonKhongLayKhongChoPhepSua</t>
+  </si>
+  <si>
+    <t>Đơn không lấy không cho phép sửa</t>
+  </si>
+  <si>
+    <t>Application not taken does not allow correction</t>
+  </si>
+  <si>
+    <t>မယူထားသော အပလီကေးရှင်းကို ပြုပြင်ခွင့်မပြုပါ။</t>
+  </si>
+  <si>
+    <t>DTTT</t>
+  </si>
+  <si>
+    <t>Payment object</t>
+  </si>
+  <si>
+    <t>ငွေပေးချေမှု ရှိကြပါတယ်။</t>
+  </si>
+  <si>
+    <t>HoSoDieuTriDangTamKhoa</t>
+  </si>
+  <si>
+    <t>Hồ sơ điều trị đang tạm khóa.</t>
+  </si>
+  <si>
+    <t>Treatment records are temporarily locked.</t>
+  </si>
+  <si>
+    <t>ကုသမှုမှတ်တမ်းများကို ယာယီသော့ခတ်ထားသည်။</t>
+  </si>
+  <si>
+    <t>HoSoGiayToDinhKem</t>
+  </si>
+  <si>
+    <t>Hồ sơ giấy tờ đính kèm</t>
+  </si>
+  <si>
+    <t>Attached documents</t>
+  </si>
+  <si>
+    <t>ပူးတွဲပါစာရွက်စာတမ်းများ</t>
+  </si>
+  <si>
+    <t>MucAn</t>
+  </si>
+  <si>
+    <t>Mức ăn</t>
+  </si>
+  <si>
+    <t>Meal level</t>
+  </si>
+  <si>
+    <t>အစားအသောက်အဆင့်</t>
+  </si>
+  <si>
+    <t>MucAnDTTT</t>
+  </si>
+  <si>
+    <t>Mức ăn/DTTT</t>
+  </si>
+  <si>
+    <t>Meal level/Payment object</t>
+  </si>
+  <si>
+    <t>အစားအသောက်အဆင့်/ငွေပေးချေမှု ရှိကြပါတယ်။</t>
+  </si>
+  <si>
+    <t>PhanLoaiBN</t>
+  </si>
+  <si>
+    <t>Phân loại bệnh nhân</t>
+  </si>
+  <si>
+    <t>Patient classification</t>
+  </si>
+  <si>
+    <t>လူနာအမျိုးအစားခွဲခြားခြင်း။</t>
+  </si>
+  <si>
+    <t>Plugins_BedRoomPartial__ToolTipCome</t>
+  </si>
+  <si>
+    <t>Bệnh nhân chuyển điều trị kết hợp từ khoa: {0}</t>
+  </si>
+  <si>
+    <t>Patient transferred to combination therapy from the department: {0}</t>
+  </si>
+  <si>
+    <t>လူနာအား ဌာနမှ ပေါင်းစပ်ကုထုံးသို့ လွှဲပြောင်းခဲ့သည်- {0}</t>
+  </si>
+  <si>
+    <t>Plugins_BedRoomPartial__ToolTipLeaves</t>
+  </si>
+  <si>
+    <t>Bệnh nhân đang điều trị kết hợp tại</t>
+  </si>
+  <si>
+    <t>Patient is on combination therapy at</t>
+  </si>
+  <si>
+    <t>လူနာသည် ပေါင်းစပ်ကုထုံးဖြင့် ကုသနေပါသည်။</t>
+  </si>
+  <si>
+    <t>TatCa</t>
+  </si>
+  <si>
+    <t>Tất cả</t>
+  </si>
+  <si>
+    <t>All</t>
+  </si>
+  <si>
+    <t>အားလုံး</t>
+  </si>
+  <si>
+    <t>ThoiGianDenPhaiLonHonThoiGianTu</t>
+  </si>
+  <si>
+    <t>Thời gian đến phải lớn hơn thời gian từ</t>
+  </si>
+  <si>
+    <t>The arrival time must be greater than the time from</t>
+  </si>
+  <si>
+    <t>ဆိုက်ရောက်ချိန်သည် အချိန်ထက် ပိုနေရမည်။</t>
+  </si>
+  <si>
+    <t>ThongBao</t>
+  </si>
+  <si>
+    <t>Thông báo</t>
+  </si>
+  <si>
+    <t>Notification</t>
+  </si>
+  <si>
+    <t>အကြောင်းကြားပါ။</t>
+  </si>
+  <si>
+    <t>ThuocVtBNDaDung</t>
+  </si>
+  <si>
+    <t>Thuốc/vt bệnh nhân đã dùng</t>
+  </si>
+  <si>
+    <t>Medications/Materails used by the patient</t>
+  </si>
+  <si>
+    <t>လူနာအသုံးပြုသော ဆေးဝါး/ပစ္စည်းများ</t>
+  </si>
+  <si>
+    <t>ToolTipDTTT</t>
+  </si>
+  <si>
+    <t>Đối tượng thanh toán</t>
+  </si>
+  <si>
+    <t>ToolTipMucAnDTTT</t>
+  </si>
+  <si>
+    <t>Mức ăn/Đối tượng thanh toán</t>
+  </si>
+  <si>
+    <t>TraSoatHoSoBenhAn</t>
+  </si>
+  <si>
+    <t>Tra soát hố sơ bệnh án</t>
+  </si>
+  <si>
+    <t>Checking the medical record hole</t>
+  </si>
+  <si>
+    <t>ဆေးမှတ်တမ်းအပေါက်ကို စစ်ဆေးခြင်း။</t>
+  </si>
+  <si>
+    <t>TrongKhoa</t>
+  </si>
+  <si>
+    <t>Trong khoa</t>
+  </si>
+  <si>
+    <t>In the faculty</t>
+  </si>
+  <si>
+    <t>ဌာနထဲမှာ</t>
+  </si>
+  <si>
+    <t>TruongDuLieuBatBuoc</t>
+  </si>
+  <si>
+    <t>Trường dữ liệu bắt buộc</t>
+  </si>
+  <si>
+    <t>Required field</t>
+  </si>
+  <si>
+    <t>လိုအပ်သောအကွက်</t>
+  </si>
+  <si>
+    <t>YLenhDaTonTaiVanBanKy</t>
+  </si>
+  <si>
+    <t>Y lệnh này đã tồn tại văn bản ký, bạn có muốn hủy dữ liệu?</t>
+  </si>
+  <si>
+    <t>This command already exists signed text, do you want to cancel the data?</t>
+  </si>
+  <si>
+    <t>ဤအမိန့်မှာ လက်မှတ်ထိုးထားသော စာသားရှိပြီး၊ သင်သည် ဒေတာကို ဖျက်လိုပါသလား။</t>
   </si>
 </sst>
 </file>
@@ -800,6 +1328,342 @@
       </c>
       <c r="F15" s="2"/>
     </row>
+    <row r="16">
+      <c r="A16" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="F16" s="2"/>
+    </row>
+    <row r="17">
+      <c r="A17" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F17" s="2"/>
+    </row>
+    <row r="18">
+      <c r="A18" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="F18" s="2"/>
+    </row>
+    <row r="19">
+      <c r="A19" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="F19" s="2"/>
+    </row>
+    <row r="20">
+      <c r="A20" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="F20" s="2"/>
+    </row>
+    <row r="21">
+      <c r="A21" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="F21" s="2"/>
+    </row>
+    <row r="22">
+      <c r="A22" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="F22" s="2"/>
+    </row>
+    <row r="23">
+      <c r="A23" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="F23" s="2"/>
+    </row>
+    <row r="24">
+      <c r="A24" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="F24" s="2"/>
+    </row>
+    <row r="25">
+      <c r="A25" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="F25" s="2"/>
+    </row>
+    <row r="26">
+      <c r="A26" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="F26" s="2"/>
+    </row>
+    <row r="27">
+      <c r="A27" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="F27" s="2"/>
+    </row>
+    <row r="28">
+      <c r="A28" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="F28" s="2"/>
+    </row>
+    <row r="29">
+      <c r="A29" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="F29" s="2"/>
+    </row>
+    <row r="30">
+      <c r="A30" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="D30" s="2"/>
+      <c r="E30" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="F30" s="2"/>
+    </row>
+    <row r="31">
+      <c r="A31" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="D31" s="2"/>
+      <c r="E31" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="F31" s="2"/>
+    </row>
+    <row r="32">
+      <c r="A32" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D32" s="2"/>
+      <c r="E32" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F32" s="2"/>
+    </row>
+    <row r="33">
+      <c r="A33" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="D33" s="2"/>
+      <c r="E33" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="F33" s="2"/>
+    </row>
+    <row r="34">
+      <c r="A34" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D34" s="2"/>
+      <c r="E34" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="F34" s="2"/>
+    </row>
+    <row r="35">
+      <c r="A35" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="D35" s="2"/>
+      <c r="E35" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="F35" s="2"/>
+    </row>
+    <row r="36">
+      <c r="A36" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="D36" s="2"/>
+      <c r="E36" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="F36" s="2"/>
+    </row>
   </sheetData>
   <pageSetup orientation="portrait"/>
 </worksheet>
@@ -838,6 +1702,502 @@
         <v>5</v>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="F2" s="2"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="F3" s="2"/>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="F4" s="2"/>
+    </row>
+    <row r="5">
+      <c r="A5" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="F5" s="2"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="F6" s="2"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="F7" s="2"/>
+    </row>
+    <row r="8">
+      <c r="A8" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="F8" s="2"/>
+    </row>
+    <row r="9">
+      <c r="A9" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="F9" s="2"/>
+    </row>
+    <row r="10">
+      <c r="A10" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="F10" s="2"/>
+    </row>
+    <row r="11">
+      <c r="A11" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="F11" s="2"/>
+    </row>
+    <row r="12">
+      <c r="A12" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="F12" s="2"/>
+    </row>
+    <row r="13">
+      <c r="A13" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="F13" s="2"/>
+    </row>
+    <row r="14">
+      <c r="A14" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="F14" s="2"/>
+    </row>
+    <row r="15">
+      <c r="A15" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="F15" s="2"/>
+    </row>
+    <row r="16">
+      <c r="A16" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="F16" s="2"/>
+    </row>
+    <row r="17">
+      <c r="A17" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="F17" s="2"/>
+    </row>
+    <row r="18">
+      <c r="A18" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="F18" s="2"/>
+    </row>
+    <row r="19">
+      <c r="A19" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="F19" s="2"/>
+    </row>
+    <row r="20">
+      <c r="A20" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="F20" s="2"/>
+    </row>
+    <row r="21">
+      <c r="A21" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="F21" s="2"/>
+    </row>
+    <row r="22">
+      <c r="A22" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="F22" s="2"/>
+    </row>
+    <row r="23">
+      <c r="A23" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="F23" s="2"/>
+    </row>
+    <row r="24">
+      <c r="A24" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="F24" s="2"/>
+    </row>
+    <row r="25">
+      <c r="A25" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="F25" s="2"/>
+    </row>
+    <row r="26">
+      <c r="A26" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="F26" s="2"/>
+    </row>
+    <row r="27">
+      <c r="A27" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="F27" s="2"/>
+    </row>
+    <row r="28">
+      <c r="A28" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="F28" s="2"/>
+    </row>
+    <row r="29">
+      <c r="A29" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="F29" s="2"/>
+    </row>
+    <row r="30">
+      <c r="A30" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="D30" s="2"/>
+      <c r="E30" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="F30" s="2"/>
+    </row>
+    <row r="31">
+      <c r="A31" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="D31" s="2"/>
+      <c r="E31" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="F31" s="2"/>
+    </row>
+    <row r="32">
+      <c r="A32" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="D32" s="2"/>
+      <c r="E32" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="F32" s="2"/>
+    </row>
   </sheetData>
   <pageSetup orientation="portrait"/>
 </worksheet>

</xml_diff>